<commit_message>
Bottle real pouring results
</commit_message>
<xml_diff>
--- a/pouring_simulation/output/results_bottle_sim_to_reality.xlsx
+++ b/pouring_simulation/output/results_bottle_sim_to_reality.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielschober/Documents/GitHub/thesis/pouring_simulation/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{ECA38B13-E404-5A43-875F-0D2F0413143D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD5E2E3-C89F-AD40-8572-C54F8216D76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary_medium_test_50_final" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="275">
   <si>
     <t>scene_number</t>
   </si>
@@ -782,12 +782,75 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>../../output/MediumBottle/Medium_370_1399_78</t>
+  </si>
+  <si>
+    <t>369.9</t>
+  </si>
+  <si>
+    <t>273.10</t>
+  </si>
+  <si>
+    <t>249.60</t>
+  </si>
+  <si>
+    <t>23.50</t>
+  </si>
+  <si>
+    <t>../../output/MediumBottle/Medium_350_1399_54</t>
+  </si>
+  <si>
+    <t>349.9</t>
+  </si>
+  <si>
+    <t>87.3</t>
+  </si>
+  <si>
+    <t>78.5</t>
+  </si>
+  <si>
+    <t>8.80</t>
+  </si>
+  <si>
+    <t>../../output/MediumBottle/Medium_430_1000_46</t>
+  </si>
+  <si>
+    <t>46.0</t>
+  </si>
+  <si>
+    <t>429.89</t>
+  </si>
+  <si>
+    <t>87.03</t>
+  </si>
+  <si>
+    <t>79.04</t>
+  </si>
+  <si>
+    <t>7.99</t>
+  </si>
+  <si>
+    <t>../../output/MediumBottle/Medium_410_1399_90</t>
+  </si>
+  <si>
+    <t>409.892</t>
+  </si>
+  <si>
+    <t>380.678</t>
+  </si>
+  <si>
+    <t>341.74</t>
+  </si>
+  <si>
+    <t>38.935</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1629,16 +1692,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="87" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="12" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="45.1640625" customWidth="1"/>
+    <col min="3" max="12" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -3651,6 +3716,238 @@
         <v>253</v>
       </c>
     </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>